<commit_message>
update values of unemployment for the new mapping
</commit_message>
<xml_diff>
--- a/xcel_data/Mapping_NEWAGE_GTAP9_18x19x4_diss.xlsx
+++ b/xcel_data/Mapping_NEWAGE_GTAP9_18x19x4_diss.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12255" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Regional Mapping" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Regional Mapping'!$B$2:$Q$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sectoral Mapping'!$A$5:$G$5</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2783,9 +2783,6 @@
     <xf numFmtId="0" fontId="18" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2796,6 +2793,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3104,9 +3104,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:XFC170"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3433,7 +3433,7 @@
         <v>212</v>
       </c>
       <c r="F4" s="120">
-        <f>IF(E4=E3,F3,F3+1)</f>
+        <f t="shared" ref="F4:F44" si="0">IF(E4=E3,F3,F3+1)</f>
         <v>2</v>
       </c>
       <c r="G4" s="120">
@@ -3574,7 +3574,7 @@
         <v>221</v>
       </c>
       <c r="F5" s="93">
-        <f>IF(E5=E4,F4,F4+1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G5" s="93">
@@ -3717,7 +3717,7 @@
         <v>233</v>
       </c>
       <c r="F6" s="95">
-        <f>IF(E6=E5,F5,F5+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G6" s="95">
@@ -3860,7 +3860,7 @@
         <v>472</v>
       </c>
       <c r="F7" s="123">
-        <f>IF(E7=E6,F6,F6+1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G7" s="123">
@@ -4005,7 +4005,7 @@
         <v>472</v>
       </c>
       <c r="F8" s="123">
-        <f>IF(E8=E7,F7,F7+1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G8" s="123">
@@ -4150,7 +4150,7 @@
         <v>241</v>
       </c>
       <c r="F9" s="103">
-        <f>IF(E9=E8,F8,F8+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G9" s="103">
@@ -4293,7 +4293,7 @@
         <v>241</v>
       </c>
       <c r="F10" s="103">
-        <f>IF(E10=E9,F9,F9+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G10" s="103">
@@ -4436,7 +4436,7 @@
         <v>585</v>
       </c>
       <c r="F11" s="94">
-        <f>IF(E11=E10,F10,F10+1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G11" s="94">
@@ -4581,7 +4581,7 @@
         <v>585</v>
       </c>
       <c r="F12" s="94">
-        <f>IF(E12=E11,F11,F11+1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G12" s="94">
@@ -4726,7 +4726,7 @@
         <v>585</v>
       </c>
       <c r="F13" s="94">
-        <f>IF(E13=E12,F12,F12+1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G13" s="94">
@@ -4871,7 +4871,7 @@
         <v>557</v>
       </c>
       <c r="F14" s="125">
-        <f>IF(E14=E13,F13,F13+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G14" s="125">
@@ -5012,7 +5012,7 @@
         <v>557</v>
       </c>
       <c r="F15" s="125">
-        <f>IF(E15=E14,F14,F14+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G15" s="125">
@@ -5153,7 +5153,7 @@
         <v>557</v>
       </c>
       <c r="F16" s="125">
-        <f>IF(E16=E15,F15,F15+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G16" s="125">
@@ -5294,7 +5294,7 @@
         <v>557</v>
       </c>
       <c r="F17" s="125">
-        <f>IF(E17=E16,F16,F16+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G17" s="125">
@@ -5435,7 +5435,7 @@
         <v>557</v>
       </c>
       <c r="F18" s="125">
-        <f>IF(E18=E17,F17,F17+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G18" s="125">
@@ -5576,7 +5576,7 @@
         <v>557</v>
       </c>
       <c r="F19" s="125">
-        <f>IF(E19=E18,F18,F18+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G19" s="125">
@@ -5717,7 +5717,7 @@
         <v>559</v>
       </c>
       <c r="F20" s="101">
-        <f>IF(E20=E19,F19,F19+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G20" s="101">
@@ -5860,7 +5860,7 @@
         <v>559</v>
       </c>
       <c r="F21" s="101">
-        <f>IF(E21=E20,F20,F20+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G21" s="101">
@@ -6003,7 +6003,7 @@
         <v>559</v>
       </c>
       <c r="F22" s="101">
-        <f>IF(E22=E21,F21,F21+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G22" s="101">
@@ -6148,7 +6148,7 @@
         <v>559</v>
       </c>
       <c r="F23" s="101">
-        <f>IF(E23=E22,F22,F22+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G23" s="101">
@@ -6291,7 +6291,7 @@
         <v>559</v>
       </c>
       <c r="F24" s="101">
-        <f>IF(E24=E23,F23,F23+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G24" s="101">
@@ -22709,7 +22709,7 @@
         <v>559</v>
       </c>
       <c r="F25" s="101">
-        <f>IF(E25=E24,F24,F24+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G25" s="101">
@@ -39127,7 +39127,7 @@
         <v>559</v>
       </c>
       <c r="F26" s="101">
-        <f>IF(E26=E25,F25,F25+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G26" s="101">
@@ -39270,7 +39270,7 @@
         <v>559</v>
       </c>
       <c r="F27" s="101">
-        <f>IF(E27=E26,F26,F26+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G27" s="101">
@@ -39413,7 +39413,7 @@
         <v>559</v>
       </c>
       <c r="F28" s="101">
-        <f>IF(E28=E27,F27,F27+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G28" s="101">
@@ -39556,7 +39556,7 @@
         <v>559</v>
       </c>
       <c r="F29" s="101">
-        <f>IF(E29=E28,F28,F28+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G29" s="101">
@@ -39699,7 +39699,7 @@
         <v>559</v>
       </c>
       <c r="F30" s="101">
-        <f>IF(E30=E29,F29,F29+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G30" s="101">
@@ -39844,7 +39844,7 @@
         <v>165</v>
       </c>
       <c r="F31" s="131">
-        <f>IF(E31=E30,F30,F30+1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G31" s="131">
@@ -39985,7 +39985,7 @@
         <v>564</v>
       </c>
       <c r="F32" s="124">
-        <f>IF(E32=E31,F31,F31+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G32" s="124">
@@ -40128,7 +40128,7 @@
         <v>564</v>
       </c>
       <c r="F33" s="124">
-        <f>IF(E33=E32,F32,F32+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G33" s="124">
@@ -40271,7 +40271,7 @@
         <v>564</v>
       </c>
       <c r="F34" s="124">
-        <f>IF(E34=E33,F33,F33+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G34" s="124">
@@ -40414,7 +40414,7 @@
         <v>564</v>
       </c>
       <c r="F35" s="124">
-        <f>IF(E35=E34,F34,F34+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G35" s="124">
@@ -40557,7 +40557,7 @@
         <v>564</v>
       </c>
       <c r="F36" s="124">
-        <f>IF(E36=E35,F35,F35+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G36" s="124">
@@ -40700,7 +40700,7 @@
         <v>564</v>
       </c>
       <c r="F37" s="124">
-        <f>IF(E37=E36,F36,F36+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G37" s="124">
@@ -40843,7 +40843,7 @@
         <v>564</v>
       </c>
       <c r="F38" s="124">
-        <f>IF(E38=E37,F37,F37+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G38" s="124">
@@ -40986,7 +40986,7 @@
         <v>564</v>
       </c>
       <c r="F39" s="124">
-        <f>IF(E39=E38,F38,F38+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G39" s="124">
@@ -41129,7 +41129,7 @@
         <v>564</v>
       </c>
       <c r="F40" s="124">
-        <f>IF(E40=E39,F39,F39+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G40" s="124">
@@ -41272,7 +41272,7 @@
         <v>564</v>
       </c>
       <c r="F41" s="124">
-        <f>IF(E41=E40,F40,F40+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G41" s="124">
@@ -41415,7 +41415,7 @@
         <v>564</v>
       </c>
       <c r="F42" s="124">
-        <f>IF(E42=E41,F41,F41+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G42" s="124">
@@ -41558,7 +41558,7 @@
         <v>564</v>
       </c>
       <c r="F43" s="124">
-        <f>IF(E43=E42,F42,F42+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G43" s="124">
@@ -41701,7 +41701,7 @@
         <v>564</v>
       </c>
       <c r="F44" s="124">
-        <f>IF(E44=E43,F43,F43+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G44" s="124">
@@ -41983,7 +41983,7 @@
         <v>260</v>
       </c>
       <c r="F46" s="126">
-        <f>IF(E46=E45,F45,F45+1)</f>
+        <f t="shared" ref="F46:F61" si="1">IF(E46=E45,F45,F45+1)</f>
         <v>13</v>
       </c>
       <c r="G46" s="126">
@@ -42124,7 +42124,7 @@
         <v>156</v>
       </c>
       <c r="F47" s="127">
-        <f>IF(E47=E46,F46,F46+1)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G47" s="127">
@@ -42265,7 +42265,7 @@
         <v>465</v>
       </c>
       <c r="F48" s="99">
-        <f>IF(E48=E47,F47,F47+1)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G48" s="99">
@@ -42406,7 +42406,7 @@
         <v>465</v>
       </c>
       <c r="F49" s="99">
-        <f>IF(E49=E48,F48,F48+1)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G49" s="99">
@@ -42547,7 +42547,7 @@
         <v>466</v>
       </c>
       <c r="F50" s="133">
-        <f>IF(E50=E49,F49,F49+1)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G50" s="133">
@@ -42688,7 +42688,7 @@
         <v>586</v>
       </c>
       <c r="F51" s="100">
-        <f>IF(E51=E50,F50,F50+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G51" s="100">
@@ -42833,7 +42833,7 @@
         <v>586</v>
       </c>
       <c r="F52" s="100">
-        <f>IF(E52=E51,F51,F51+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G52" s="100">
@@ -42976,7 +42976,7 @@
         <v>586</v>
       </c>
       <c r="F53" s="100">
-        <f>IF(E53=E52,F52,F52+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G53" s="100">
@@ -43121,7 +43121,7 @@
         <v>586</v>
       </c>
       <c r="F54" s="100">
-        <f>IF(E54=E53,F53,F53+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G54" s="100">
@@ -43266,7 +43266,7 @@
         <v>586</v>
       </c>
       <c r="F55" s="100">
-        <f>IF(E55=E54,F54,F54+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G55" s="100">
@@ -43411,7 +43411,7 @@
         <v>586</v>
       </c>
       <c r="F56" s="100">
-        <f>IF(E56=E55,F55,F55+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G56" s="100">
@@ -43556,7 +43556,7 @@
         <v>586</v>
       </c>
       <c r="F57" s="100">
-        <f>IF(E57=E56,F56,F56+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G57" s="100">
@@ -43701,7 +43701,7 @@
         <v>586</v>
       </c>
       <c r="F58" s="100">
-        <f>IF(E58=E57,F57,F57+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G58" s="100">
@@ -43844,7 +43844,7 @@
         <v>586</v>
       </c>
       <c r="F59" s="100">
-        <f>IF(E59=E58,F58,F58+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G59" s="100">
@@ -43989,7 +43989,7 @@
         <v>586</v>
       </c>
       <c r="F60" s="100">
-        <f>IF(E60=E59,F59,F59+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G60" s="100">
@@ -44134,7 +44134,7 @@
         <v>586</v>
       </c>
       <c r="F61" s="100">
-        <f>IF(E61=E60,F60,F60+1)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G61" s="100">
@@ -44706,7 +44706,7 @@
         <v>586</v>
       </c>
       <c r="F65" s="100">
-        <f>IF(E65=E64,F64,F64+1)</f>
+        <f t="shared" ref="F65:F96" si="2">IF(E65=E64,F64,F64+1)</f>
         <v>17</v>
       </c>
       <c r="G65" s="100">
@@ -44736,10 +44736,10 @@
       <c r="O65" s="100" t="s">
         <v>483</v>
       </c>
-      <c r="P65" s="158" t="s">
+      <c r="P65" s="157" t="s">
         <v>571</v>
       </c>
-      <c r="Q65" s="158" t="s">
+      <c r="Q65" s="157" t="s">
         <v>583</v>
       </c>
       <c r="R65" s="85"/>
@@ -44851,7 +44851,7 @@
         <v>586</v>
       </c>
       <c r="F66" s="100">
-        <f>IF(E66=E65,F65,F65+1)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G66" s="100">
@@ -44881,10 +44881,10 @@
       <c r="O66" s="100" t="s">
         <v>483</v>
       </c>
-      <c r="P66" s="159" t="s">
+      <c r="P66" s="158" t="s">
         <v>571</v>
       </c>
-      <c r="Q66" s="158" t="s">
+      <c r="Q66" s="157" t="s">
         <v>583</v>
       </c>
       <c r="R66" s="49"/>
@@ -44996,7 +44996,7 @@
         <v>586</v>
       </c>
       <c r="F67" s="100">
-        <f>IF(E67=E66,F66,F66+1)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="G67" s="100">
@@ -45026,8 +45026,8 @@
       <c r="O67" s="100" t="s">
         <v>483</v>
       </c>
-      <c r="P67" s="160"/>
-      <c r="Q67" s="161" t="s">
+      <c r="P67" s="159"/>
+      <c r="Q67" s="160" t="s">
         <v>584</v>
       </c>
       <c r="R67" s="49"/>
@@ -45139,7 +45139,7 @@
         <v>532</v>
       </c>
       <c r="F68" s="98">
-        <f>IF(E68=E67,F67,F67+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G68" s="98">
@@ -45282,7 +45282,7 @@
         <v>532</v>
       </c>
       <c r="F69" s="98">
-        <f>IF(E69=E68,F68,F68+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G69" s="98">
@@ -45425,7 +45425,7 @@
         <v>532</v>
       </c>
       <c r="F70" s="98">
-        <f>IF(E70=E69,F69,F69+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G70" s="98">
@@ -45568,7 +45568,7 @@
         <v>532</v>
       </c>
       <c r="F71" s="98">
-        <f>IF(E71=E70,F70,F70+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G71" s="98">
@@ -45711,7 +45711,7 @@
         <v>532</v>
       </c>
       <c r="F72" s="98">
-        <f>IF(E72=E71,F71,F71+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G72" s="98">
@@ -45854,7 +45854,7 @@
         <v>532</v>
       </c>
       <c r="F73" s="98">
-        <f>IF(E73=E72,F72,F72+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G73" s="98">
@@ -45997,7 +45997,7 @@
         <v>532</v>
       </c>
       <c r="F74" s="153">
-        <f>IF(E74=E73,F73,F73+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G74" s="153">
@@ -46142,7 +46142,7 @@
         <v>532</v>
       </c>
       <c r="F75" s="98">
-        <f>IF(E75=E74,F74,F74+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G75" s="98">
@@ -46285,7 +46285,7 @@
         <v>532</v>
       </c>
       <c r="F76" s="98">
-        <f>IF(E76=E75,F75,F75+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G76" s="98">
@@ -46428,7 +46428,7 @@
         <v>532</v>
       </c>
       <c r="F77" s="153">
-        <f>IF(E77=E76,F76,F76+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G77" s="153">
@@ -46573,7 +46573,7 @@
         <v>532</v>
       </c>
       <c r="F78" s="153">
-        <f>IF(E78=E77,F77,F77+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G78" s="153">
@@ -46718,7 +46718,7 @@
         <v>532</v>
       </c>
       <c r="F79" s="98">
-        <f>IF(E79=E78,F78,F78+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G79" s="98">
@@ -46861,7 +46861,7 @@
         <v>532</v>
       </c>
       <c r="F80" s="98">
-        <f>IF(E80=E79,F79,F79+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G80" s="98">
@@ -47004,7 +47004,7 @@
         <v>532</v>
       </c>
       <c r="F81" s="98">
-        <f>IF(E81=E80,F80,F80+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G81" s="98">
@@ -47147,7 +47147,7 @@
         <v>532</v>
       </c>
       <c r="F82" s="98">
-        <f>IF(E82=E81,F81,F81+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G82" s="98">
@@ -47290,7 +47290,7 @@
         <v>532</v>
       </c>
       <c r="F83" s="98">
-        <f>IF(E83=E82,F82,F82+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G83" s="98">
@@ -47433,7 +47433,7 @@
         <v>532</v>
       </c>
       <c r="F84" s="98">
-        <f>IF(E84=E83,F83,F83+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G84" s="98">
@@ -47576,7 +47576,7 @@
         <v>532</v>
       </c>
       <c r="F85" s="153">
-        <f>IF(E85=E84,F84,F84+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G85" s="153">
@@ -47721,7 +47721,7 @@
         <v>532</v>
       </c>
       <c r="F86" s="98">
-        <f>IF(E86=E85,F85,F85+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G86" s="98">
@@ -47864,7 +47864,7 @@
         <v>532</v>
       </c>
       <c r="F87" s="98">
-        <f>IF(E87=E86,F86,F86+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G87" s="98">
@@ -48007,7 +48007,7 @@
         <v>532</v>
       </c>
       <c r="F88" s="98">
-        <f>IF(E88=E87,F87,F87+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G88" s="98">
@@ -48150,7 +48150,7 @@
         <v>532</v>
       </c>
       <c r="F89" s="98">
-        <f>IF(E89=E88,F88,F88+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G89" s="98">
@@ -48293,7 +48293,7 @@
         <v>532</v>
       </c>
       <c r="F90" s="98">
-        <f>IF(E90=E89,F89,F89+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G90" s="98">
@@ -48436,7 +48436,7 @@
         <v>532</v>
       </c>
       <c r="F91" s="153">
-        <f>IF(E91=E90,F90,F90+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G91" s="153">
@@ -48581,7 +48581,7 @@
         <v>532</v>
       </c>
       <c r="F92" s="98">
-        <f>IF(E92=E91,F91,F91+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G92" s="98">
@@ -48724,7 +48724,7 @@
         <v>532</v>
       </c>
       <c r="F93" s="98">
-        <f>IF(E93=E92,F92,F92+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G93" s="98">
@@ -48867,7 +48867,7 @@
         <v>532</v>
       </c>
       <c r="F94" s="153">
-        <f>IF(E94=E93,F93,F93+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G94" s="153">
@@ -49012,7 +49012,7 @@
         <v>532</v>
       </c>
       <c r="F95" s="153">
-        <f>IF(E95=E94,F94,F94+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G95" s="153">
@@ -49157,7 +49157,7 @@
         <v>532</v>
       </c>
       <c r="F96" s="98">
-        <f>IF(E96=E95,F95,F95+1)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="G96" s="98">
@@ -49300,7 +49300,7 @@
         <v>532</v>
       </c>
       <c r="F97" s="98">
-        <f>IF(E97=E96,F96,F96+1)</f>
+        <f t="shared" ref="F97:F128" si="3">IF(E97=E96,F96,F96+1)</f>
         <v>18</v>
       </c>
       <c r="G97" s="98">
@@ -49443,7 +49443,7 @@
         <v>532</v>
       </c>
       <c r="F98" s="98">
-        <f>IF(E98=E97,F97,F97+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G98" s="98">
@@ -49586,7 +49586,7 @@
         <v>532</v>
       </c>
       <c r="F99" s="98">
-        <f>IF(E99=E98,F98,F98+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G99" s="98">
@@ -49729,7 +49729,7 @@
         <v>532</v>
       </c>
       <c r="F100" s="98">
-        <f>IF(E100=E99,F99,F99+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G100" s="98">
@@ -49872,7 +49872,7 @@
         <v>532</v>
       </c>
       <c r="F101" s="98">
-        <f>IF(E101=E100,F100,F100+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G101" s="98">
@@ -50015,7 +50015,7 @@
         <v>532</v>
       </c>
       <c r="F102" s="98">
-        <f>IF(E102=E101,F101,F101+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G102" s="98">
@@ -50158,7 +50158,7 @@
         <v>532</v>
       </c>
       <c r="F103" s="98">
-        <f>IF(E103=E102,F102,F102+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G103" s="98">
@@ -50301,7 +50301,7 @@
         <v>532</v>
       </c>
       <c r="F104" s="98">
-        <f>IF(E104=E103,F103,F103+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G104" s="98">
@@ -50444,7 +50444,7 @@
         <v>532</v>
       </c>
       <c r="F105" s="98">
-        <f>IF(E105=E104,F104,F104+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G105" s="98">
@@ -50587,7 +50587,7 @@
         <v>532</v>
       </c>
       <c r="F106" s="98">
-        <f>IF(E106=E105,F105,F105+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G106" s="98">
@@ -50730,7 +50730,7 @@
         <v>532</v>
       </c>
       <c r="F107" s="98">
-        <f>IF(E107=E106,F106,F106+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G107" s="98">
@@ -50873,7 +50873,7 @@
         <v>532</v>
       </c>
       <c r="F108" s="98">
-        <f>IF(E108=E107,F107,F107+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G108" s="98">
@@ -51016,7 +51016,7 @@
         <v>532</v>
       </c>
       <c r="F109" s="98">
-        <f>IF(E109=E108,F108,F108+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G109" s="98">
@@ -51159,7 +51159,7 @@
         <v>532</v>
       </c>
       <c r="F110" s="98">
-        <f>IF(E110=E109,F109,F109+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G110" s="98">
@@ -51302,7 +51302,7 @@
         <v>532</v>
       </c>
       <c r="F111" s="98">
-        <f>IF(E111=E110,F110,F110+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G111" s="98">
@@ -51445,7 +51445,7 @@
         <v>532</v>
       </c>
       <c r="F112" s="98">
-        <f>IF(E112=E111,F111,F111+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G112" s="98">
@@ -51588,7 +51588,7 @@
         <v>532</v>
       </c>
       <c r="F113" s="98">
-        <f>IF(E113=E112,F112,F112+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G113" s="98">
@@ -51731,7 +51731,7 @@
         <v>532</v>
       </c>
       <c r="F114" s="153">
-        <f>IF(E114=E113,F113,F113+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G114" s="153">
@@ -51876,7 +51876,7 @@
         <v>532</v>
       </c>
       <c r="F115" s="98">
-        <f>IF(E115=E114,F114,F114+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G115" s="98">
@@ -52019,7 +52019,7 @@
         <v>532</v>
       </c>
       <c r="F116" s="98">
-        <f>IF(E116=E115,F115,F115+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G116" s="98">
@@ -52162,7 +52162,7 @@
         <v>532</v>
       </c>
       <c r="F117" s="98">
-        <f>IF(E117=E116,F116,F116+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G117" s="98">
@@ -52305,7 +52305,7 @@
         <v>532</v>
       </c>
       <c r="F118" s="98">
-        <f>IF(E118=E117,F117,F117+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G118" s="98">
@@ -52448,7 +52448,7 @@
         <v>532</v>
       </c>
       <c r="F119" s="98">
-        <f>IF(E119=E118,F118,F118+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G119" s="98">
@@ -52591,7 +52591,7 @@
         <v>532</v>
       </c>
       <c r="F120" s="98">
-        <f>IF(E120=E119,F119,F119+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G120" s="98">
@@ -52734,7 +52734,7 @@
         <v>532</v>
       </c>
       <c r="F121" s="98">
-        <f>IF(E121=E120,F120,F120+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G121" s="98">
@@ -52877,7 +52877,7 @@
         <v>532</v>
       </c>
       <c r="F122" s="98">
-        <f>IF(E122=E121,F121,F121+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G122" s="98">
@@ -53020,7 +53020,7 @@
         <v>532</v>
       </c>
       <c r="F123" s="98">
-        <f>IF(E123=E122,F122,F122+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G123" s="98">
@@ -53163,7 +53163,7 @@
         <v>532</v>
       </c>
       <c r="F124" s="98">
-        <f>IF(E124=E123,F123,F123+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G124" s="98">
@@ -53306,7 +53306,7 @@
         <v>532</v>
       </c>
       <c r="F125" s="98">
-        <f>IF(E125=E124,F124,F124+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G125" s="98">
@@ -53449,7 +53449,7 @@
         <v>532</v>
       </c>
       <c r="F126" s="98">
-        <f>IF(E126=E125,F125,F125+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G126" s="98">
@@ -53592,7 +53592,7 @@
         <v>532</v>
       </c>
       <c r="F127" s="98">
-        <f>IF(E127=E126,F126,F126+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G127" s="98">
@@ -53733,7 +53733,7 @@
         <v>532</v>
       </c>
       <c r="F128" s="98">
-        <f>IF(E128=E127,F127,F127+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="G128" s="98">
@@ -53876,7 +53876,7 @@
         <v>532</v>
       </c>
       <c r="F129" s="98">
-        <f>IF(E129=E128,F128,F128+1)</f>
+        <f t="shared" ref="F129:F160" si="4">IF(E129=E128,F128,F128+1)</f>
         <v>18</v>
       </c>
       <c r="G129" s="98">
@@ -54019,7 +54019,7 @@
         <v>532</v>
       </c>
       <c r="F130" s="153">
-        <f>IF(E130=E129,F129,F129+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G130" s="153">
@@ -54164,7 +54164,7 @@
         <v>532</v>
       </c>
       <c r="F131" s="98">
-        <f>IF(E131=E130,F130,F130+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G131" s="98">
@@ -54307,7 +54307,7 @@
         <v>532</v>
       </c>
       <c r="F132" s="98">
-        <f>IF(E132=E131,F131,F131+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G132" s="98">
@@ -54450,7 +54450,7 @@
         <v>532</v>
       </c>
       <c r="F133" s="98">
-        <f>IF(E133=E132,F132,F132+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G133" s="98">
@@ -54593,7 +54593,7 @@
         <v>532</v>
       </c>
       <c r="F134" s="98">
-        <f>IF(E134=E133,F133,F133+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G134" s="98">
@@ -54736,7 +54736,7 @@
         <v>532</v>
       </c>
       <c r="F135" s="98">
-        <f>IF(E135=E134,F134,F134+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G135" s="98">
@@ -54879,7 +54879,7 @@
         <v>532</v>
       </c>
       <c r="F136" s="98">
-        <f>IF(E136=E135,F135,F135+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G136" s="98">
@@ -55022,7 +55022,7 @@
         <v>532</v>
       </c>
       <c r="F137" s="98">
-        <f>IF(E137=E136,F136,F136+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G137" s="98">
@@ -55165,7 +55165,7 @@
         <v>532</v>
       </c>
       <c r="F138" s="153">
-        <f>IF(E138=E137,F137,F137+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G138" s="153">
@@ -55310,7 +55310,7 @@
         <v>532</v>
       </c>
       <c r="F139" s="153">
-        <f>IF(E139=E138,F138,F138+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G139" s="153">
@@ -55455,7 +55455,7 @@
         <v>532</v>
       </c>
       <c r="F140" s="98">
-        <f>IF(E140=E139,F139,F139+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G140" s="98">
@@ -55598,7 +55598,7 @@
         <v>532</v>
       </c>
       <c r="F141" s="98">
-        <f>IF(E141=E140,F140,F140+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G141" s="98">
@@ -55741,7 +55741,7 @@
         <v>532</v>
       </c>
       <c r="F142" s="98">
-        <f>IF(E142=E141,F141,F141+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G142" s="98">
@@ -55884,7 +55884,7 @@
         <v>532</v>
       </c>
       <c r="F143" s="98">
-        <f>IF(E143=E142,F142,F142+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G143" s="98">
@@ -56027,7 +56027,7 @@
         <v>532</v>
       </c>
       <c r="F144" s="98">
-        <f>IF(E144=E143,F143,F143+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G144" s="98">
@@ -56170,7 +56170,7 @@
         <v>532</v>
       </c>
       <c r="F145" s="98">
-        <f>IF(E145=E144,F144,F144+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G145" s="98">
@@ -56313,7 +56313,7 @@
         <v>532</v>
       </c>
       <c r="F146" s="156">
-        <f>IF(E146=E145,F145,F145+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G146" s="156">
@@ -56454,7 +56454,7 @@
         <v>532</v>
       </c>
       <c r="F147" s="156">
-        <f>IF(E147=E146,F146,F146+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G147" s="156">
@@ -56595,7 +56595,7 @@
         <v>532</v>
       </c>
       <c r="F148" s="156">
-        <f>IF(E148=E147,F147,F147+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G148" s="156">
@@ -56643,7 +56643,7 @@
         <v>532</v>
       </c>
       <c r="F149" s="156">
-        <f>IF(E149=E148,F148,F148+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G149" s="156">
@@ -56691,7 +56691,7 @@
         <v>532</v>
       </c>
       <c r="F150" s="156">
-        <f>IF(E150=E149,F149,F149+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G150" s="156">
@@ -56739,7 +56739,7 @@
         <v>532</v>
       </c>
       <c r="F151" s="156">
-        <f>IF(E151=E150,F150,F150+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G151" s="156">
@@ -56787,7 +56787,7 @@
         <v>532</v>
       </c>
       <c r="F152" s="156">
-        <f>IF(E152=E151,F151,F151+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G152" s="156">
@@ -56835,7 +56835,7 @@
         <v>532</v>
       </c>
       <c r="F153" s="156">
-        <f>IF(E153=E152,F152,F152+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G153" s="156">
@@ -56883,7 +56883,7 @@
         <v>532</v>
       </c>
       <c r="F154" s="156">
-        <f>IF(E154=E153,F153,F153+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G154" s="156">
@@ -56931,7 +56931,7 @@
         <v>532</v>
       </c>
       <c r="F155" s="156">
-        <f>IF(E155=E154,F154,F154+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G155" s="156">
@@ -56979,7 +56979,7 @@
         <v>532</v>
       </c>
       <c r="F156" s="156">
-        <f>IF(E156=E155,F155,F155+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G156" s="156">
@@ -57027,7 +57027,7 @@
         <v>532</v>
       </c>
       <c r="F157" s="156">
-        <f>IF(E157=E156,F156,F156+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G157" s="156">
@@ -57075,7 +57075,7 @@
         <v>532</v>
       </c>
       <c r="F158" s="156">
-        <f>IF(E158=E157,F157,F157+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G158" s="156">
@@ -57123,7 +57123,7 @@
         <v>532</v>
       </c>
       <c r="F159" s="156">
-        <f>IF(E159=E158,F158,F158+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G159" s="156">
@@ -57171,7 +57171,7 @@
         <v>532</v>
       </c>
       <c r="F160" s="156">
-        <f>IF(E160=E159,F159,F159+1)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G160" s="156">
@@ -57219,7 +57219,7 @@
         <v>532</v>
       </c>
       <c r="F161" s="156">
-        <f>IF(E161=E160,F160,F160+1)</f>
+        <f t="shared" ref="F161:F192" si="5">IF(E161=E160,F160,F160+1)</f>
         <v>18</v>
       </c>
       <c r="G161" s="156">
@@ -57267,7 +57267,7 @@
         <v>532</v>
       </c>
       <c r="F162" s="156">
-        <f>IF(E162=E161,F161,F161+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G162" s="156">
@@ -57315,7 +57315,7 @@
         <v>532</v>
       </c>
       <c r="F163" s="156">
-        <f>IF(E163=E162,F162,F162+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G163" s="156">
@@ -57363,7 +57363,7 @@
         <v>532</v>
       </c>
       <c r="F164" s="156">
-        <f>IF(E164=E163,F163,F163+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G164" s="156">
@@ -57411,7 +57411,7 @@
         <v>532</v>
       </c>
       <c r="F165" s="156">
-        <f>IF(E165=E164,F164,F164+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G165" s="156">
@@ -57459,7 +57459,7 @@
         <v>532</v>
       </c>
       <c r="F166" s="156">
-        <f>IF(E166=E165,F165,F165+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G166" s="156">
@@ -57507,7 +57507,7 @@
         <v>532</v>
       </c>
       <c r="F167" s="156">
-        <f>IF(E167=E166,F166,F166+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G167" s="156">
@@ -57555,7 +57555,7 @@
         <v>532</v>
       </c>
       <c r="F168" s="156">
-        <f>IF(E168=E167,F167,F167+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G168" s="156">
@@ -57603,7 +57603,7 @@
         <v>532</v>
       </c>
       <c r="F169" s="156">
-        <f>IF(E169=E168,F168,F168+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G169" s="156">
@@ -57651,7 +57651,7 @@
         <v>532</v>
       </c>
       <c r="F170" s="156">
-        <f>IF(E170=E169,F169,F169+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="G170" s="156">
@@ -57701,8 +57701,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A2:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57733,16 +57733,16 @@
       <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="157" t="s">
+      <c r="A4" s="161" t="s">
         <v>486</v>
       </c>
-      <c r="B4" s="157"/>
+      <c r="B4" s="161"/>
       <c r="C4" s="14"/>
-      <c r="D4" s="157" t="s">
+      <c r="D4" s="161" t="s">
         <v>487</v>
       </c>
-      <c r="E4" s="157"/>
-      <c r="F4" s="157"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -63688,16 +63688,16 @@
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="161" t="s">
         <v>486</v>
       </c>
-      <c r="B3" s="157"/>
+      <c r="B3" s="161"/>
       <c r="C3" s="14"/>
-      <c r="D3" s="157" t="s">
+      <c r="D3" s="161" t="s">
         <v>487</v>
       </c>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">

</xml_diff>